<commit_message>
Copied and renamed classes.
</commit_message>
<xml_diff>
--- a/GP3 Diagrams/StateTransitionTable.xlsx
+++ b/GP3 Diagrams/StateTransitionTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\OneDrive\Desktop\Eclipse Workspace\Git\ICS_372-Group_Project\GP3 Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D5184A7-76FB-4113-9935-5C7172D0C1B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F580F09-689C-4587-A947-865EAEC6C219}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{894B0C3F-CD1C-40C3-97F8-F29793698F5D}"/>
+    <workbookView xWindow="384" yWindow="0" windowWidth="17280" windowHeight="6852" xr2:uid="{894B0C3F-CD1C-40C3-97F8-F29793698F5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="17">
   <si>
     <t>Fan</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Ideal Temp + 3</t>
   </si>
   <si>
-    <t>Timer @ 10</t>
-  </si>
-  <si>
     <t>Air Conditioner</t>
   </si>
   <si>
@@ -79,6 +76,12 @@
   </si>
   <si>
     <t>Heater Idle</t>
+  </si>
+  <si>
+    <t>Ideal Temperature</t>
+  </si>
+  <si>
+    <t>TimerAt10</t>
   </si>
 </sst>
 </file>
@@ -432,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7800F54-54B0-41A8-A4CF-1920881424F2}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,10 +455,10 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -475,10 +478,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -492,16 +495,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -515,16 +518,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -544,10 +547,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -564,16 +567,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -582,7 +585,7 @@
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -593,10 +596,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -616,118 +619,118 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -738,10 +741,10 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -767,10 +770,10 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added Thermometer. Change a few text in the GUI. Deleted unnecessary events.
</commit_message>
<xml_diff>
--- a/GP3 Diagrams/StateTransitionTable.xlsx
+++ b/GP3 Diagrams/StateTransitionTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnp82\Documents\GitHub\ICS_372-Group_Project\GP3 Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1859CBBD-2E4B-4D15-830F-2778A8B09E1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AF0D41-2F42-4ADF-8C04-0C253AEEC034}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="3" xr2:uid="{894B0C3F-CD1C-40C3-97F8-F29793698F5D}"/>
+    <workbookView minimized="1" xWindow="8400" yWindow="345" windowWidth="10800" windowHeight="7380" xr2:uid="{894B0C3F-CD1C-40C3-97F8-F29793698F5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Transition table" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -352,15 +352,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,19 +693,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7800F54-54B0-41A8-A4CF-1920881424F2}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="3" max="3" width="9.6796875" customWidth="1"/>
-    <col min="4" max="4" width="19.08984375" customWidth="1"/>
+    <col min="4" max="4" width="16.90625" customWidth="1"/>
     <col min="6" max="6" width="17.86328125" customWidth="1"/>
-    <col min="7" max="7" width="21.86328125" customWidth="1"/>
-    <col min="8" max="8" width="15.31640625" customWidth="1"/>
-    <col min="9" max="9" width="18.76953125" customWidth="1"/>
+    <col min="7" max="7" width="16.953125" customWidth="1"/>
+    <col min="8" max="8" width="13.86328125" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
     <col min="10" max="10" width="12.1328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -806,236 +822,244 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" t="s">
-        <v>7</v>
-      </c>
+      <c r="F9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="J15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1275,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D909839-65F9-4D67-A145-D7D15C161096}">
   <dimension ref="A2:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>